<commit_message>
Merged PR 9553: BP-848 : Display results in Excel export - formatting update
Fixed column formatting
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - PlanQuote.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - PlanQuote.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6C4015-F679-4BBA-A4E5-6A8E22B81573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885348C7-0C78-4FBF-B2F3-C0A5729DD806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="435" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27375" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rate Details" sheetId="1" r:id="rId1"/>
@@ -82,11 +82,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -147,7 +148,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -156,6 +157,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -488,7 +490,7 @@
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="8">
         <f>SUM(I8:I9)</f>
         <v>0</v>
       </c>
@@ -551,10 +553,8 @@
       <c r="G8" s="4">
         <v>0</v>
       </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
+      <c r="H8" s="5"/>
+      <c r="I8" s="8">
         <f>H8*L8</f>
         <v>0</v>
       </c>
@@ -581,10 +581,8 @@
       <c r="G9" s="4">
         <v>0</v>
       </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
+      <c r="H9" s="5"/>
+      <c r="I9" s="8">
         <f>H9*L9</f>
         <v>0</v>
       </c>
@@ -592,8 +590,20 @@
         <f>H9*M9</f>
         <v>0</v>
       </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Entry must be a whole number." sqref="H8:H9" xr:uid="{8F822E32-9CFB-4C88-B1EB-B96115521224}">
+      <formula1>1</formula1>
+      <formula2>999999999999999000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>